<commit_message>
added votes to Goshen 2000 R primary file
</commit_message>
<xml_diff>
--- a/raw/20000822/GO-R-2000.xlsx
+++ b/raw/20000822/GO-R-2000.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="201" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="201"/>
   </bookViews>
   <sheets>
-    <sheet name="A" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>Total</t>
   </si>
@@ -138,38 +142,23 @@
   </si>
   <si>
     <t>Official Totals</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="2"/>
@@ -181,6 +170,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +194,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -199,86 +202,376 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:IF31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:240">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -514,7 +807,7 @@
       <c r="HK1" s="1"/>
       <c r="HL1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:240">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -750,7 +1043,7 @@
       <c r="HK2" s="1"/>
       <c r="HL2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:240">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -992,7 +1285,7 @@
       <c r="IE3" s="1"/>
       <c r="IF3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:240">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -1252,7 +1545,7 @@
       <c r="IE4" s="1"/>
       <c r="IF4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:240">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1268,79 +1561,151 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:240">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="5">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
+        <v>30</v>
+      </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="E6" s="5">
+        <v>27</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="K6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:240">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="5">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
+        <v>29</v>
+      </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="5">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:240">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5">
+        <v>162</v>
+      </c>
+      <c r="C8" s="5">
+        <v>156</v>
+      </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="E8" s="5">
+        <v>122</v>
+      </c>
+      <c r="F8" s="5">
+        <v>24</v>
+      </c>
+      <c r="G8" s="5">
+        <v>9</v>
+      </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="5">
+        <v>145</v>
+      </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="K8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N8" s="5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:240">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="5">
+        <v>76</v>
+      </c>
+      <c r="C9" s="5">
+        <v>71</v>
+      </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="E9" s="5">
+        <v>56</v>
+      </c>
+      <c r="F9" s="5">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5">
+        <v>60</v>
+      </c>
       <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N9" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:240">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1356,97 +1721,187 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:240">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="5">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5">
+        <v>17</v>
+      </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="E11" s="5">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2</v>
+      </c>
       <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="5">
+        <v>15</v>
+      </c>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:240">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="5">
+        <v>102</v>
+      </c>
+      <c r="C12" s="5">
+        <v>97</v>
+      </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="E12" s="5">
+        <v>78</v>
+      </c>
+      <c r="F12" s="5">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5">
+        <v>3</v>
+      </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="5">
+        <v>80</v>
+      </c>
       <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N12" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:240">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="5">
+        <v>98</v>
+      </c>
+      <c r="C13" s="5">
+        <v>90</v>
+      </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="5">
+        <v>57</v>
+      </c>
+      <c r="F13" s="5">
+        <v>28</v>
+      </c>
+      <c r="G13" s="5">
+        <v>6</v>
+      </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="5">
+        <v>80</v>
+      </c>
       <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:240">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="5">
+        <v>179</v>
+      </c>
+      <c r="C14" s="5">
+        <v>162</v>
+      </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="E14" s="5">
+        <v>118</v>
+      </c>
+      <c r="F14" s="5">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5">
+        <v>6</v>
+      </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="K14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="5">
+        <v>140</v>
+      </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:240">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="5">
+        <v>93</v>
+      </c>
+      <c r="C15" s="5">
+        <v>87</v>
+      </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="5">
+        <v>66</v>
+      </c>
+      <c r="F15" s="5">
+        <v>16</v>
+      </c>
+      <c r="G15" s="5">
+        <v>4</v>
+      </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="K15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="5">
+        <v>64</v>
+      </c>
       <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:240">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1462,97 +1917,187 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:14">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="5">
+        <v>174</v>
+      </c>
+      <c r="C17" s="5">
+        <v>159</v>
+      </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="E17" s="5">
+        <v>127</v>
+      </c>
+      <c r="F17" s="5">
+        <v>36</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
       <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="5">
+        <v>146</v>
+      </c>
       <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="5">
+        <v>128</v>
+      </c>
+      <c r="C18" s="5">
+        <v>119</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="E18" s="5">
+        <v>91</v>
+      </c>
+      <c r="F18" s="5">
+        <v>25</v>
+      </c>
+      <c r="G18" s="5">
+        <v>3</v>
+      </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="K18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" s="5">
+        <v>107</v>
+      </c>
       <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="5">
+        <v>95</v>
+      </c>
+      <c r="C19" s="5">
+        <v>88</v>
+      </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="E19" s="5">
+        <v>75</v>
+      </c>
+      <c r="F19" s="5">
+        <v>11</v>
+      </c>
+      <c r="G19" s="5">
+        <v>7</v>
+      </c>
       <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="K19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="5">
+        <v>79</v>
+      </c>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="5">
+        <v>165</v>
+      </c>
+      <c r="C20" s="5">
+        <v>157</v>
+      </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="E20" s="5">
+        <v>118</v>
+      </c>
+      <c r="F20" s="5">
+        <v>34</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5</v>
+      </c>
       <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="5">
+        <v>139</v>
+      </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N20" s="5">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="5">
+        <v>61</v>
+      </c>
+      <c r="C21" s="5">
+        <v>57</v>
+      </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="E21" s="5">
+        <v>47</v>
+      </c>
+      <c r="F21" s="5">
+        <v>11</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="K21" s="5">
+        <v>52</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N21" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1568,79 +2113,151 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:14">
       <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="5">
+        <v>38</v>
+      </c>
+      <c r="C23" s="5">
+        <v>37</v>
+      </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="E23" s="5">
+        <v>32</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>3</v>
+      </c>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="K23" s="5">
+        <v>36</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="5">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5">
+        <v>47</v>
+      </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="5">
+        <v>38</v>
+      </c>
+      <c r="F24" s="5">
+        <v>9</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="I24" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="K24" s="5">
+        <v>42</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N24" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="5">
+        <v>87</v>
+      </c>
+      <c r="C25" s="5">
+        <v>79</v>
+      </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="E25" s="5">
+        <v>65</v>
+      </c>
+      <c r="F25" s="5">
+        <v>11</v>
+      </c>
+      <c r="G25" s="5">
+        <v>3</v>
+      </c>
       <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" s="5">
+        <v>72</v>
+      </c>
       <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N25" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="5">
+        <v>52</v>
+      </c>
+      <c r="C26" s="5">
+        <v>52</v>
+      </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="E26" s="5">
+        <v>42</v>
+      </c>
+      <c r="F26" s="5">
+        <v>7</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
       <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="I26" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="K26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" s="5">
+        <v>48</v>
+      </c>
       <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N26" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1656,43 +2273,79 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:14">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="5">
+        <v>108</v>
+      </c>
+      <c r="C28" s="5">
+        <v>102</v>
+      </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="5">
+        <v>75</v>
+      </c>
+      <c r="F28" s="5">
+        <v>18</v>
+      </c>
+      <c r="G28" s="5">
+        <v>4</v>
+      </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="K28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="5">
+        <v>97</v>
+      </c>
       <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N28" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="5">
+        <v>15</v>
+      </c>
+      <c r="C29" s="5">
+        <v>14</v>
+      </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="5">
+        <v>13</v>
+      </c>
+      <c r="F29" s="5">
+        <v>2</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="K29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="5">
+        <v>14</v>
+      </c>
       <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N29" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1708,58 +2361,62 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="5" t="n">
-        <f aca="false">SUM(B6:B29)</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="2" t="n">
-        <f aca="false">SUM(C6:C29)</f>
-        <v>0</v>
+      <c r="B31" s="5">
+        <f>SUM(B6:B29)</f>
+        <v>1760</v>
+      </c>
+      <c r="C31" s="2">
+        <f>SUM(C6:C29)</f>
+        <v>1650</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="2" t="n">
-        <f aca="false">SUM(E6:E29)</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="5" t="n">
-        <f aca="false">SUM(F6:F29)</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="5" t="n">
-        <f aca="false">SUM(G6:G29)</f>
-        <v>0</v>
+      <c r="E31" s="2">
+        <f>SUM(E6:E29)</f>
+        <v>1280</v>
+      </c>
+      <c r="F31" s="5">
+        <f>SUM(F6:F29)</f>
+        <v>310</v>
+      </c>
+      <c r="G31" s="5">
+        <f>SUM(G6:G29)</f>
+        <v>69</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="2" t="n">
-        <f aca="false">SUM(I6:I29)</f>
-        <v>0</v>
+      <c r="I31" s="2">
+        <f>SUM(I6:I29)</f>
+        <v>344</v>
       </c>
       <c r="J31" s="5"/>
-      <c r="K31" s="2" t="n">
-        <f aca="false">SUM(K6:K29)</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="2" t="n">
-        <f aca="false">SUM(L6:L29)</f>
-        <v>0</v>
+      <c r="K31" s="2">
+        <f>SUM(K6:K29)</f>
+        <v>130</v>
+      </c>
+      <c r="L31" s="2">
+        <f>SUM(L6:L29)</f>
+        <v>942</v>
       </c>
       <c r="M31" s="5"/>
-      <c r="N31" s="2" t="n">
-        <f aca="false">SUM(N6:N29)</f>
-        <v>0</v>
+      <c r="N31" s="2">
+        <f>SUM(N6:N29)</f>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>